<commit_message>
Remove text_value. Do explicit string conversions.
CVDLS-176
</commit_message>
<xml_diff>
--- a/tests/Entity/workbooks/workbook.xlsx
+++ b/tests/Entity/workbooks/workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/Entity/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D503BE2-B6E4-FF4C-94D4-1B8DAC73EB2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8718DB6E-44F2-6149-849A-E31849640BE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="540" windowWidth="22020" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PVE690RLR_ra_calls" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>SpecimenQPCRResults1</t>
   </si>
@@ -39,21 +39,20 @@
   <si>
     <t>Text</t>
   </si>
-  <si>
-    <t>Rounded Decimal</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="169" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="170" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="172" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="173" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.000000000000000000000000000"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +189,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -542,16 +548,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -907,81 +916,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="8"/>
-    <col min="8" max="9" width="12.83203125" style="8" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="8"/>
-    <col min="11" max="12" width="11.83203125" style="8" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="7"/>
+    <col min="8" max="9" width="12.83203125" style="7" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="7"/>
+    <col min="11" max="12" width="11.83203125" style="7" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>43904.681018518517</v>
       </c>
-      <c r="C2" s="3">
-        <v>20.439682831841399</v>
-      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>43904.722685185188</v>
       </c>
-      <c r="C3" s="3">
-        <v>18.893144729852999</v>
-      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>43904.764351851853</v>
       </c>
-      <c r="C4" s="3">
-        <v>19.621005213173898</v>
-      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>43904.806018518517</v>
       </c>
-      <c r="C5" s="3">
-        <v>21.987654320000001</v>
-      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
Excel Import system supports TRUE / FALSE as boolean true / false
CVDLS-220
CVDLS-60
</commit_message>
<xml_diff>
--- a/tests/Entity/workbooks/workbook.xlsx
+++ b/tests/Entity/workbooks/workbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/Entity/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8718DB6E-44F2-6149-849A-E31849640BE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5C601D-2037-2444-AECE-43BF894E4106}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>SpecimenQPCRResults1</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>Text</t>
+  </si>
+  <si>
+    <t>True / False</t>
   </si>
 </sst>
 </file>
@@ -919,7 +922,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -944,7 +947,9 @@
       <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="11"/>
+      <c r="C1" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -954,7 +959,9 @@
       <c r="B2" s="4">
         <v>43904.681018518517</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="D2" s="10"/>
       <c r="E2" s="8"/>
     </row>
@@ -965,7 +972,9 @@
       <c r="B3" s="3">
         <v>43904.722685185188</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="11" t="b">
+        <v>0</v>
+      </c>
       <c r="D3" s="11"/>
       <c r="E3" s="9"/>
     </row>
@@ -976,7 +985,9 @@
       <c r="B4" s="5">
         <v>43904.764351851853</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="11" t="b">
+        <v>0</v>
+      </c>
       <c r="D4" s="11"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -986,7 +997,9 @@
       <c r="B5" s="6">
         <v>43904.806018518517</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>